<commit_message>
première série de modifications
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOSSIER USER\GIANNI\bureau\Openclassrooms\Projet 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOSSIER USER\GIANNI\bureau\Openclassrooms\Projet 4\MaquetteS Projet 4\P4_raimondo_gianni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2A57E9-5D40-426F-A63C-69BA0C70FC1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C8950D-FBF0-45B3-84B7-14648DC9EDC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29595" yWindow="2130" windowWidth="21600" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="1770" windowWidth="27645" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>Catégorie</t>
   </si>
@@ -98,13 +98,166 @@
   </si>
   <si>
     <t>Mettre le nom de l'agence</t>
+  </si>
+  <si>
+    <t>valeur attribut "lang" balise &lt;html&gt; en "défaut"</t>
+  </si>
+  <si>
+    <t>l'attribut "lang" doit etre defini par une langue</t>
+  </si>
+  <si>
+    <t>balise meta keyword</t>
+  </si>
+  <si>
+    <t>à supprimer</t>
+  </si>
+  <si>
+    <t>balise meta description, content vide</t>
+  </si>
+  <si>
+    <t>mettre une description</t>
+  </si>
+  <si>
+    <t>balises scriptS L15 à L19</t>
+  </si>
+  <si>
+    <t>black hat</t>
+  </si>
+  <si>
+    <t>il faut une description, phrase d'accroche</t>
+  </si>
+  <si>
+    <t>Mettre le nom de l'agence ou complément</t>
+  </si>
+  <si>
+    <t>mettre "async" ou "defer"</t>
+  </si>
+  <si>
+    <t>manque ordre exe script (important/pas important)</t>
+  </si>
+  <si>
+    <t>mettre fr car site en français</t>
+  </si>
+  <si>
+    <t>manque H2 dans structure titre</t>
+  </si>
+  <si>
+    <t>il faut un H2 avant un H3</t>
+  </si>
+  <si>
+    <t>alt des images non correspondantes</t>
+  </si>
+  <si>
+    <t>alt en mode "keyword"</t>
+  </si>
+  <si>
+    <t>modifier les alt</t>
+  </si>
+  <si>
+    <t>images trop grandes</t>
+  </si>
+  <si>
+    <t>images plus grande que leur conteneurs</t>
+  </si>
+  <si>
+    <t>redimmensionné ou compressé les images</t>
+  </si>
+  <si>
+    <t>1 et 2</t>
+  </si>
+  <si>
+    <t>contraste</t>
+  </si>
+  <si>
+    <t>validation de contraste</t>
+  </si>
+  <si>
+    <t>réadapter les contrastes</t>
+  </si>
+  <si>
+    <t>texte à 1px</t>
+  </si>
+  <si>
+    <t>image à la place de texte</t>
+  </si>
+  <si>
+    <t>H1 meme couleur que le fond</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>Agence de Développement Web Sur-mesure</t>
+  </si>
+  <si>
+    <t>selon vos Besoins et votre Métier</t>
+  </si>
+  <si>
+    <t>basé sur Lyon, faites appel à notre expertise pour créer ou améliorer</t>
+  </si>
+  <si>
+    <t>votre visibilité numérique,</t>
+  </si>
+  <si>
+    <t>Agence de Développement Web Sur-mesure basé sur Lyon, faites appel à notre expertise pour créer ou améliorer votre visibilité numérique, selon vos Besoins et votre Métier.</t>
+  </si>
+  <si>
+    <t>Balise bouton L45 caché et inutile</t>
+  </si>
+  <si>
+    <t>rien ne ressort dans le CSS et sur le site</t>
+  </si>
+  <si>
+    <t>Toggle navigation + liens accueil &amp; page 2 inutiles</t>
+  </si>
+  <si>
+    <t>inutiles</t>
+  </si>
+  <si>
+    <t>Nom du lien vers page 2</t>
+  </si>
+  <si>
+    <t>Nom du lien inadéquate</t>
+  </si>
+  <si>
+    <t>Modifier par "Contact"</t>
+  </si>
+  <si>
+    <t>restructurer les balises titres dans l'ordre</t>
+  </si>
+  <si>
+    <t>code special pour caractere special</t>
+  </si>
+  <si>
+    <t>modifié le code par le caractere</t>
+  </si>
+  <si>
+    <t>encodage meta charset en utf-8</t>
+  </si>
+  <si>
+    <t>Photo de texte à la place de texte = trop lourd</t>
+  </si>
+  <si>
+    <t>remettre du texte à la place des images</t>
+  </si>
+  <si>
+    <t>Pas de liens vers réseaux sociaux de l'entreprise</t>
+  </si>
+  <si>
+    <t>Liens réseaux sociaux entreprise redirigé vers page accueil</t>
+  </si>
+  <si>
+    <t>Créer des comptes de réseaux sociaux pour la société ou (si déjà fait), les ajouter</t>
+  </si>
+  <si>
+    <t>https://www.alsacreations.com/astuce/lire/1166-alt-title-images-liens.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +297,42 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -178,14 +367,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,197 +630,541 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="4"/>
+    <col min="2" max="2" width="21.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="43.21875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="40" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" style="11" customWidth="1"/>
     <col min="8" max="27" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="b">
+      <c r="F5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="b">
+      <c r="C11" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="4" t="b">
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:27" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:27" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="4" t="b">
+      <c r="G17" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="4" t="b">
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="4" t="b">
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="4" t="b">
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="4" t="b">
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.2">
+      <c r="C31" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1544,9 +2117,19 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifications des images, alt et dimensions
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOSSIER USER\GIANNI\bureau\Openclassrooms\Projet 4\MaquetteS Projet 4\P4_raimondo_gianni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C8950D-FBF0-45B3-84B7-14648DC9EDC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A63466A-2F75-4F11-AE7C-17D7144CAF2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="1770" windowWidth="27645" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="210" windowWidth="27645" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Catégorie</t>
   </si>
@@ -160,9 +160,6 @@
     <t>images plus grande que leur conteneurs</t>
   </si>
   <si>
-    <t>redimmensionné ou compressé les images</t>
-  </si>
-  <si>
     <t>1 et 2</t>
   </si>
   <si>
@@ -184,24 +181,15 @@
     <t>H1 meme couleur que le fond</t>
   </si>
   <si>
-    <t>Fait</t>
-  </si>
-  <si>
     <t>Agence de Développement Web Sur-mesure</t>
   </si>
   <si>
     <t>selon vos Besoins et votre Métier</t>
   </si>
   <si>
-    <t>basé sur Lyon, faites appel à notre expertise pour créer ou améliorer</t>
-  </si>
-  <si>
     <t>votre visibilité numérique,</t>
   </si>
   <si>
-    <t>Agence de Développement Web Sur-mesure basé sur Lyon, faites appel à notre expertise pour créer ou améliorer votre visibilité numérique, selon vos Besoins et votre Métier.</t>
-  </si>
-  <si>
     <t>Balise bouton L45 caché et inutile</t>
   </si>
   <si>
@@ -247,10 +235,28 @@
     <t>Liens réseaux sociaux entreprise redirigé vers page accueil</t>
   </si>
   <si>
-    <t>Créer des comptes de réseaux sociaux pour la société ou (si déjà fait), les ajouter</t>
-  </si>
-  <si>
     <t>https://www.alsacreations.com/astuce/lire/1166-alt-title-images-liens.html</t>
+  </si>
+  <si>
+    <t>balise form</t>
+  </si>
+  <si>
+    <t>à faire</t>
+  </si>
+  <si>
+    <t>Effectué</t>
+  </si>
+  <si>
+    <t>Créer des comptes de réseaux sociaux pour la société ou (si déjà Effectué), les ajouter</t>
+  </si>
+  <si>
+    <t>basé sur Lyon, Effectuées appel à notre expertise pour créer ou améliorer</t>
+  </si>
+  <si>
+    <t>Agence de Développement Web Sur-mesure basé sur Lyon, Effectuées appel à notre expertise pour créer ou améliorer votre visibilité numérique, selon vos Besoins et votre Métier.</t>
+  </si>
+  <si>
+    <t>convertir, redimmensionner ou compresser les images</t>
   </si>
 </sst>
 </file>
@@ -633,7 +639,7 @@
   <dimension ref="A1:AA1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD25"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -642,7 +648,7 @@
     <col min="2" max="2" width="21.33203125" style="8" customWidth="1"/>
     <col min="3" max="3" width="43.21875" style="8" customWidth="1"/>
     <col min="4" max="4" width="40" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" style="8" customWidth="1"/>
     <col min="7" max="7" width="27.109375" style="11" customWidth="1"/>
     <col min="8" max="27" width="10.5546875" customWidth="1"/>
@@ -693,7 +699,7 @@
     </row>
     <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>9</v>
@@ -708,13 +714,13 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>9</v>
@@ -729,13 +735,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>9</v>
@@ -750,7 +756,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G4" s="12"/>
     </row>
@@ -771,7 +777,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G5" s="12"/>
     </row>
@@ -792,7 +798,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G6" s="12"/>
     </row>
@@ -812,8 +818,8 @@
       <c r="E7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="b">
-        <v>0</v>
+      <c r="F7" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G7" s="12"/>
     </row>
@@ -825,7 +831,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>20</v>
@@ -834,7 +840,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G8" s="12"/>
     </row>
@@ -846,16 +852,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G9" s="12"/>
     </row>
@@ -867,16 +873,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G10" s="12"/>
     </row>
@@ -888,16 +894,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G11" s="12"/>
     </row>
@@ -915,10 +921,10 @@
         <v>27</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G12" s="12"/>
     </row>
@@ -930,16 +936,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="G13" s="12"/>
     </row>
@@ -951,133 +957,108 @@
         <v>9</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="13" t="b">
-        <v>0</v>
+      <c r="F14" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:27" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:27" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+    <row r="15" spans="1:27" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="C21" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="13" t="b">
-        <v>0</v>
-      </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1094,28 +1075,33 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="13" t="b">
-        <v>0</v>
+      <c r="F24" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>2</v>
+      </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="C25" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="13" t="b">
-        <v>0</v>
+      <c r="F25" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G25" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C27" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="8">
         <v>33</v>
@@ -1123,7 +1109,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E28" s="8">
         <v>57</v>
@@ -1131,10 +1117,10 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" s="8">
         <v>52</v>
@@ -1143,7 +1129,7 @@
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modif responsive pages 1 & 2
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOSSIER USER\GIANNI\bureau\Openclassrooms\Projet 4\MaquetteS Projet 4\P4_raimondo_gianni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A63466A-2F75-4F11-AE7C-17D7144CAF2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF77C67-BDEC-45BF-BE16-6DB742B9C88B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="210" windowWidth="27645" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-(SEO ou accessiblité ?)</t>
+(SEO, accessiblité, bonne pratique ou performance)</t>
         </r>
       </text>
     </comment>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>Catégorie</t>
   </si>
@@ -257,13 +257,40 @@
   </si>
   <si>
     <t>convertir, redimmensionner ou compresser les images</t>
+  </si>
+  <si>
+    <t>accessibilité</t>
+  </si>
+  <si>
+    <t>enumerer les blocs</t>
+  </si>
+  <si>
+    <t>remis</t>
+  </si>
+  <si>
+    <t>href erroné sur balise link</t>
+  </si>
+  <si>
+    <t>les fichiers ne sont pas rattaché à l'HTML</t>
+  </si>
+  <si>
+    <t>Déclarer les bonnes adresses "locals"</t>
+  </si>
+  <si>
+    <t>Bonnes Pratiques</t>
+  </si>
+  <si>
+    <t>https://www.anthedesign.fr/referencement/backlink/#:~:text=Obtenir%20des%20backlinks%20de%20qualit%C3%A9,page%20similaire%20sans%20liens%20entrants</t>
+  </si>
+  <si>
+    <t>Liens footer de mauvaise qualité et non pertinent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,6 +366,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -373,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -419,6 +457,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -636,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1009"/>
+  <dimension ref="A1:AA1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -761,20 +808,20 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>12</v>
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>61</v>
@@ -783,43 +830,43 @@
     </row>
     <row r="6" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="G7" s="12"/>
     </row>
@@ -830,17 +877,17 @@
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>37</v>
+      <c r="C8" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>61</v>
+        <v>23</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G8" s="12"/>
     </row>
@@ -848,14 +895,14 @@
       <c r="A9" s="4">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>44</v>
+      <c r="C9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
@@ -866,41 +913,41 @@
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="18">
         <v>1</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>61</v>
+      <c r="C10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>61</v>
@@ -909,19 +956,19 @@
     </row>
     <row r="12" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>50</v>
+      <c r="C12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>61</v>
@@ -932,68 +979,66 @@
       <c r="A13" s="4">
         <v>1</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>61</v>
       </c>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>1</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>56</v>
+      <c r="C14" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:27" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>1</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="C15" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:27" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -1001,87 +1046,118 @@
         <v>9</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="G16" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>1</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="C22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>2</v>
-      </c>
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
-      <c r="C24" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
@@ -1089,8 +1165,8 @@
         <v>2</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="12" t="s">
-        <v>59</v>
+      <c r="C25" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -1099,58 +1175,60 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="9" t="s">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>2</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="8">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="8">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="2" t="s">
+    </row>
+    <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="8">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="37" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+      <c r="C38" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-    </row>
-    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2112,6 +2190,7 @@
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
ajout liens réseaux sociaux
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOSSIER USER\GIANNI\bureau\Openclassrooms\Projet 4\MaquetteS Projet 4\P4_raimondo_gianni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B0999C-2C25-487B-B293-6E43843F407C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78526D4D-34CB-48C3-AB43-781AF83B8878}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="120" windowWidth="28170" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>Balise meta keyword</t>
   </si>
   <si>
-    <t>"href" erroné sur balise &lt;link&gt;</t>
-  </si>
-  <si>
     <t>Pas de titre sur onglet</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve">Images plus grandes que leur conteneurs, trop riche en poids et au format </t>
+  </si>
+  <si>
+    <t>Adresse local "href" erronée sur balise &lt;link&gt;</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
   <dimension ref="A1:AA1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -791,10 +791,10 @@
         <v>47</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>23</v>
@@ -812,10 +812,10 @@
         <v>48</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>23</v>
@@ -851,10 +851,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>28</v>
@@ -872,10 +872,10 @@
         <v>29</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>9</v>
@@ -893,7 +893,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>8</v>
@@ -914,13 +914,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>22</v>
@@ -935,13 +935,13 @@
         <v>29</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>23</v>
@@ -977,13 +977,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>23</v>
@@ -998,13 +998,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>23</v>
@@ -1037,16 +1037,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>23</v>
@@ -1060,16 +1060,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>89</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>23</v>
@@ -1088,7 +1088,7 @@
         <v>31</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>23</v>
@@ -1102,7 +1102,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>40</v>
@@ -1125,13 +1125,13 @@
         <v>29</v>
       </c>
       <c r="C18" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="E18" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>86</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>23</v>
@@ -1143,13 +1143,13 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>23</v>
@@ -1198,13 +1198,13 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>23</v>
@@ -1223,7 +1223,7 @@
         <v>39</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>23</v>
@@ -1240,10 +1240,10 @@
         <v>34</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>23</v>
@@ -1257,19 +1257,19 @@
         <v>11</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>59</v>
+        <v>79</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>22</v>
+        <v>78</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
dernières modifs maquettes et finalisation document audit
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOSSIER USER\GIANNI\bureau\Openclassrooms\Projet 4\MaquetteS Projet 4\P4_raimondo_gianni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78526D4D-34CB-48C3-AB43-781AF83B8878}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F58EF82-1304-4453-8BC7-94CD0704B666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Gianni Raimondo</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5E6EE245-8BD4-41E9-8AC0-BD95010444E1}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5E6EE245-8BD4-41E9-8AC0-BD95010444E1}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Catégorie</t>
   </si>
@@ -79,259 +79,199 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>Page</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
-    <t>"page 2" au lieu d'un titre</t>
-  </si>
-  <si>
-    <t>Mettre le nom de l'agence</t>
-  </si>
-  <si>
-    <t>Mettre le nom de l'agence ou complément</t>
-  </si>
-  <si>
-    <t>1 et 2</t>
-  </si>
-  <si>
-    <t>Agence de Développement Web Sur-mesure</t>
-  </si>
-  <si>
-    <t>selon vos Besoins et votre Métier</t>
-  </si>
-  <si>
-    <t>votre visibilité numérique,</t>
-  </si>
-  <si>
-    <t>Nom du lien vers page 2</t>
-  </si>
-  <si>
-    <t>Nom du lien inadéquate</t>
-  </si>
-  <si>
-    <t>Modifier par "Contact"</t>
-  </si>
-  <si>
-    <t>Photo de texte à la place de texte = trop lourd</t>
-  </si>
-  <si>
-    <t>Pas de liens vers réseaux sociaux de l'entreprise</t>
-  </si>
-  <si>
-    <t>Liens réseaux sociaux entreprise redirigé vers page accueil</t>
-  </si>
-  <si>
     <t>https://www.alsacreations.com/astuce/lire/1166-alt-title-images-liens.html</t>
   </si>
   <si>
     <t>à faire</t>
   </si>
   <si>
-    <t>Effectué</t>
-  </si>
-  <si>
-    <t>Créer des comptes de réseaux sociaux pour la société ou (si déjà Effectué), les ajouter</t>
-  </si>
-  <si>
-    <t>basé sur Lyon, Effectuées appel à notre expertise pour créer ou améliorer</t>
-  </si>
-  <si>
-    <t>Agence de Développement Web Sur-mesure basé sur Lyon, Effectuées appel à notre expertise pour créer ou améliorer votre visibilité numérique, selon vos Besoins et votre Métier.</t>
-  </si>
-  <si>
-    <t>enumerer les blocs</t>
-  </si>
-  <si>
-    <t>Déclarer les bonnes adresses "locals"</t>
-  </si>
-  <si>
     <t>Bonnes Pratiques</t>
   </si>
   <si>
     <t>https://www.anthedesign.fr/referencement/backlink/#:~:text=Obtenir%20des%20backlinks%20de%20qualit%C3%A9,page%20similaire%20sans%20liens%20entrants</t>
   </si>
   <si>
-    <t>Liens footer de mauvaise qualité et non pertinent</t>
-  </si>
-  <si>
-    <t>H1 invisible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact mail des coordonnées </t>
-  </si>
-  <si>
-    <t>"Coordonnées" HTML mal écrites</t>
-  </si>
-  <si>
-    <t>Taille de la police trop petite</t>
-  </si>
-  <si>
-    <t>Il faut une description, phrase d'accroche</t>
-  </si>
-  <si>
-    <t>Mettre une description</t>
-  </si>
-  <si>
-    <t>"content" de la balise &lt;meta-description&gt; vide</t>
-  </si>
-  <si>
-    <t>Pas de mise en place d'envoi de mail au clic sur contact</t>
-  </si>
-  <si>
-    <t>Taille police</t>
-  </si>
-  <si>
-    <t>"src" de la balise &lt;script&gt; erroné</t>
-  </si>
-  <si>
-    <t>QFGDIUHQDSFGPIOUHQDSF</t>
-  </si>
-  <si>
-    <t>SDFVBHÖQDFIHGSDFB</t>
-  </si>
-  <si>
-    <t>Correction des "src", conforme aux fichiers</t>
-  </si>
-  <si>
-    <t>Les "src" ne correspondent pas aux noms des fichiers</t>
-  </si>
-  <si>
-    <t>Supprimer du parametrage taile police des balises &lt;p&gt; dans le CSS</t>
-  </si>
-  <si>
-    <t>Valeur attribut "lang" balise &lt;html&gt; en "défaut"</t>
-  </si>
-  <si>
-    <t>Balise meta keyword</t>
-  </si>
-  <si>
-    <t>Pas de titre sur onglet</t>
-  </si>
-  <si>
-    <t>Mauvais nom d'onglet</t>
-  </si>
-  <si>
-    <t>Balises scriptS L15 à L19</t>
-  </si>
-  <si>
-    <t>Texte à 1px</t>
-  </si>
-  <si>
-    <t>Manque H2 dans structure titre</t>
-  </si>
-  <si>
-    <t>Image à la place de texte</t>
-  </si>
-  <si>
-    <t>"alt" des images non correspondants</t>
-  </si>
-  <si>
-    <t>Code special pour caractere special</t>
-  </si>
-  <si>
-    <t>Attributs de la balise form</t>
-  </si>
-  <si>
-    <t>Contraste</t>
-  </si>
-  <si>
-    <t>L'attribut "lang" doit etre defini par une langue</t>
-  </si>
-  <si>
-    <t>Black hat</t>
-  </si>
-  <si>
-    <t>Les fichiers ne sont pas rattaché à l'HTML</t>
-  </si>
-  <si>
-    <t>Un point sur la balise Title au lieu du nom</t>
-  </si>
-  <si>
     <t>Manque ordre d'execution script (important/pas important)</t>
   </si>
   <si>
-    <t>Il faut un H2 avant un H3</t>
-  </si>
-  <si>
-    <t>"alt" en mode "keyword"</t>
-  </si>
-  <si>
-    <t>Encodage meta charset en utf-8</t>
-  </si>
-  <si>
-    <t>"success-msg" et "fail-msg" non valide et en erreur au validateur</t>
-  </si>
-  <si>
-    <t>Manque balise "address"</t>
-  </si>
-  <si>
-    <t>Validation de contraste</t>
-  </si>
-  <si>
-    <t>Mettre "fr" car site en français</t>
-  </si>
-  <si>
-    <t>À supprimer</t>
-  </si>
-  <si>
-    <t>Mettre "async" ou "defer"</t>
-  </si>
-  <si>
-    <t>Restructurer les balises titres dans l'ordre</t>
-  </si>
-  <si>
-    <t>Remettre du texte à la place des images</t>
-  </si>
-  <si>
-    <t>Modifié le code spéciaux par le caractere</t>
-  </si>
-  <si>
-    <t>"href" déclaré en "mailto" sur le contact</t>
-  </si>
-  <si>
-    <t>Remplacer la div encadrante par la balise address</t>
-  </si>
-  <si>
-    <t>Réadapter les contrastes</t>
-  </si>
-  <si>
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>Modifier les "alt"</t>
-  </si>
-  <si>
     <t>Performance</t>
   </si>
   <si>
-    <t>Accessibilité / Bonnes Pratiques</t>
-  </si>
-  <si>
-    <t>Manques balises sémantiques</t>
-  </si>
-  <si>
-    <t>Manques les balises &lt;header&gt;, &lt;main&gt;, &lt;section&gt; et &lt;footer&gt;</t>
-  </si>
-  <si>
-    <t>Structurer le code HTML avec des balsies sémantiques</t>
-  </si>
-  <si>
-    <t>Accessibilité / SEO</t>
-  </si>
-  <si>
-    <t>Images de trop grande taille, trop lourdes et au mauvais formats</t>
-  </si>
-  <si>
-    <t>Convertir, redimmensionner et/ou compresser les images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Images plus grandes que leur conteneurs, trop riche en poids et au format </t>
-  </si>
-  <si>
-    <t>Adresse local "href" erronée sur balise &lt;link&gt;</t>
+    <t>L'attribut "content" de la balise &lt;meta - description&gt; est vide</t>
+  </si>
+  <si>
+    <t>Le texte de la description n'est pas renseigné</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/la-balise-meta-keywords/</t>
+  </si>
+  <si>
+    <t>Présence de la balise &lt;meta - keyword&gt;</t>
+  </si>
+  <si>
+    <t>La présence de cette balise est considéré comme du Black hat</t>
+  </si>
+  <si>
+    <t>Ne pas mettre en place la balise &lt;meta - keyword&gt;</t>
+  </si>
+  <si>
+    <t>Supprimer la balise &lt;meta - keyword&gt;</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/metadonnee-description-2/</t>
+  </si>
+  <si>
+    <t>Mettre une description à l'attribut "content" de la balise &lt;meta&gt; de maximum 160 caractères</t>
+  </si>
+  <si>
+    <t>Remplacement de la description actuelle (en mode répétition de mot clé =&gt; pratique de blackhat) par une déscription précise avec le mot clé principal</t>
+  </si>
+  <si>
+    <t>L'attribut "alt" des balises &lt;img&gt; ne sont pas conformes</t>
+  </si>
+  <si>
+    <t>L'attribut "alt" a été déclaré en répétition de "mots clés" au lieu d'une description de l'image à laquelle il est rattaché</t>
+  </si>
+  <si>
+    <t>L'attribut "alt de la balise &lt;img&gt; doit décrire l'image qu'il accompagne</t>
+  </si>
+  <si>
+    <t>Remplacement de la description actuelle (en mode répétition de mot clé =&gt; pratique de blackhat) par une déscription se rapportant à l'image</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/html/html5_semantic_elements.asp</t>
+  </si>
+  <si>
+    <t>Manque la balise &lt;H2&gt; dans la structure des  titres de la page 1 "Accueil", ainsi que des balises sémantiques (&lt;header&gt;, &lt;footer&gt;, &lt;main&gt;, &lt;section&gt;, etc…) dans les 2 pages HTML</t>
+  </si>
+  <si>
+    <t>La mise en place des balises entête &lt;H1 à H6&gt; présente le manque de la balise &lt;H2&gt; sur la page 1 "accueil", et le code HTML des 2 pages n'est pas construit avec les balises sémantiques adaptés</t>
+  </si>
+  <si>
+    <t>Les balises entêtes doivent se suivre lors du developpement du code, et des balises sémantiques doivent être utilisées</t>
+  </si>
+  <si>
+    <t>Insertion d'une balise &lt;H2&gt; dans la structure des titres de la page 1 "Accueil", ainsi que des balises sémantiques &lt;header&gt;, &lt;footer&gt;, &lt;main&gt;, &gt;section&gt; pour une meilleur structure du code dans les 2 pages</t>
+  </si>
+  <si>
+    <t>Du texte "mots clés" à 1px a été placé comme bordure supérieur et inférieur au logo, les textes des boutons, de certains titres et paragraphes sont trop clairs voir invisibles, et les liens des réseaux sociaux n'ont pas de texte visible et renvoi tous sur la page "Accueil"</t>
+  </si>
+  <si>
+    <t>Eviter la pratique "black hat" d'insertion de micro-texte "mots clés", utiliser de bonnes couleurs de police pour une meilleure visibilité, et paramétrer les liens avec les bonnes adresses, avec un texte / titre ou un label</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
+  </si>
+  <si>
+    <t>Mauvais contraste sur le logo, les boutons, les liens, et certains titres et textes; les liens n'ont pas de noms visibles</t>
+  </si>
+  <si>
+    <t>Valeur de l'attribut "lang" de la balise &lt;html&gt;  non paramétrée</t>
+  </si>
+  <si>
+    <t>L'attribut "lang" doit être defini par une langue et non avec la valeur "defaut"</t>
+  </si>
+  <si>
+    <t>Définir la langue du site en relation avec le pays par la bonne valeur de l'attribut "lang" de la balise &lt;html&gt;</t>
+  </si>
+  <si>
+    <t>Ajout de la valeur "fr" à l'attribut "lang" de la balise &lt;html&gt; sur les 2 pages</t>
+  </si>
+  <si>
+    <t>https://yesyouweb.com/pourquoi-comment-optimiser-images-site-web/</t>
+  </si>
+  <si>
+    <t>Images de trop grande taille, trop lourdes et au mauvais formats; et "image-texte" à la place de texte</t>
+  </si>
+  <si>
+    <t>Images plus grandes que leur conteneurs, trop riche en poids (octets) et au format non adaptés (bmp); "image-texte" plus longue à charger car une image est plus lourde qu'un texte</t>
+  </si>
+  <si>
+    <t>Convertir, redimmensionner et/ou compresser les images, utiliser du texte au lieu d'une image quand cela est possible</t>
+  </si>
+  <si>
+    <t>Images redimentionnées, converties et compressées, et "image-texte" remplacées par du texte</t>
+  </si>
+  <si>
+    <t>Entreprise webdesign Lyon</t>
+  </si>
+  <si>
+    <t>Les liens de la balise &lt;footer&gt; ne sont pas pertinents</t>
+  </si>
+  <si>
+    <t>Les liens de la balise &lt;footer&gt; ne sont pas en adéquation avec l'activité proposé par l'entreprise</t>
+  </si>
+  <si>
+    <t>Mettre en place des liens moins nombreux mais plus cohérent en rapport avec le service proposé par la société</t>
+  </si>
+  <si>
+    <t>Suppression des liens hors rapport avec l'agence</t>
+  </si>
+  <si>
+    <t>Validateur en erreur sur la balise &lt;form&gt;</t>
+  </si>
+  <si>
+    <t>Les attributs "success-msg" et "fail-msg"ne sont pas tolérés et déclenche une erreur au validateur</t>
+  </si>
+  <si>
+    <t>Utiliser les bons attributs correspondants aux balises</t>
+  </si>
+  <si>
+    <t>Suppression des attributs erronés</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/html/html_forms_attributes.asp</t>
+  </si>
+  <si>
+    <t>Les textes du code HTML présentent des "codes" spéciaux pour des "caractères speciaux", les balises &lt;title&gt; sont inadaptées et l'adresse mail de la société en page 2 n'est pas un lien</t>
+  </si>
+  <si>
+    <t>https://www.jchr.be/html/caracteres.htm
+https://developer.mozilla.org/fr/docs/Web/HTML/Element/title
+https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/Creating_hyperlinks</t>
+  </si>
+  <si>
+    <t>La balise &lt;meta &gt; encodée en "charset utf-8" nous permet d'utiliser les "caractères spéciaux" à la place de "codes" spéciaux, les balise &lt;title&gt; font apparaître des noms d'onglets inadéquates, et l'adresse mail de la page 2 "Contact" est un paragraphe</t>
+  </si>
+  <si>
+    <t>Modification des "codes" spéciaux par les caractères spéciaux voulus, insertion des bons noms / mots pour les onglets, et paramétrage de l'adresse mail en "envoi de courrier éléctronique" au clic sur l'adresse mail</t>
+  </si>
+  <si>
+    <t>Utiliser un encodage adapté et éviter les "codes" spéciaux substitutifs, appliquer les bons noms / mots à la balise &lt;title&gt;, et utiliser la balise &lt;a&gt; avec l'attribut "href-mailto" en cas d'adresse mail sur le site</t>
+  </si>
+  <si>
+    <t>Suppression du micro-texte, modification de la couleur de police de certains éléments, redirection des liens "réseaux sociaux" vers leurs pages d'accueil et ajout d'un "aria-label" sur chacun;
+Ajouts d' "aria-label" supplémentaires</t>
+  </si>
+  <si>
+    <t>Attributs d'importances sur les balises &lt;script&gt;</t>
+  </si>
+  <si>
+    <t>Mettre un attribut "async" ou "defer"</t>
+  </si>
+  <si>
+    <t>Pas de CDN mis en place</t>
+  </si>
+  <si>
+    <t>Vitesse de chargement de la page moins rapide</t>
+  </si>
+  <si>
+    <t>Etudier la pertinence de la mise en place d'un CDN selon les critères de trafic (importance), de spams (attaque), des ressources statiques (images)</t>
+  </si>
+  <si>
+    <t>https://www.ovh.com/fr/cdn/avantages.xml</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/tag_script.asp</t>
   </si>
 </sst>
 </file>
@@ -358,11 +298,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -403,24 +338,31 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +375,14 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -449,63 +397,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -719,601 +753,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1009"/>
+  <dimension ref="A1:Z1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="4"/>
-    <col min="2" max="2" width="20.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="40" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" style="11" customWidth="1"/>
-    <col min="8" max="27" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="41.77734375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="47.5546875" style="6" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="11.21875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" s="7" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
+      <c r="B2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:26" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="7" customFormat="1" ht="81" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="7" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:26" ht="60" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="12"/>
+      <c r="D14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="12"/>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="9"/>
     </row>
-    <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="12"/>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="5"/>
     </row>
-    <row r="5" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="12"/>
+    <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
     </row>
-    <row r="6" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="12"/>
+    <row r="25" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="6"/>
     </row>
-    <row r="7" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="12"/>
+    <row r="26" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="6"/>
     </row>
-    <row r="8" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="12"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="11"/>
     </row>
-    <row r="9" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="12"/>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="12"/>
     </row>
-    <row r="10" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>1</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="12"/>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="12"/>
+      <c r="C38" s="11"/>
+      <c r="F38" s="1"/>
     </row>
-    <row r="11" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="12"/>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13"/>
+      <c r="B40" s="12"/>
     </row>
-    <row r="12" spans="1:27" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>1</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:27" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>1</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:27" ht="90" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>2</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>2</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>2</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="17">
-        <v>2</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>2</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2275,10 +2078,27 @@
     <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{B6729B59-15FE-42E4-990F-5C4283A93ADD}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{654C40A6-BD04-4183-9268-49CBDA637277}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{8BA5BDAC-C805-4CEE-9F80-4B77D1FFE22B}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{21178044-D4A4-4B87-8788-53A4316B998E}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{C6D855C0-1152-4F75-BE7A-63F955D1B5C7}"/>
+    <hyperlink ref="F5" r:id="rId6" location=":~:text=Obtenir%20des%20backlinks%20de%20qualit%C3%A9,page%20similaire%20sans%20liens%20entrants" xr:uid="{068FDCEF-6393-4581-969D-2A4E65F0A232}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{5F399373-37D8-4C9C-A280-8A7520C58BFA}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{558B7B29-AD54-4F1C-95AD-FAD9555D8755}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{EF58D68C-7882-4D41-BA52-05B618DC1787}"/>
+    <hyperlink ref="F11" r:id="rId10" display="https://www.jchr.be/html/caracteres.htm" xr:uid="{1A6C42CB-FC7C-4E11-8AE9-DAAF2909DA35}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{E4F62578-716A-4F11-8534-12F07CC3DF8F}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{D41031DE-5E20-4F96-B1AC-8845714175DB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>